<commit_message>
Updated the app list and added a Version column
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F5405E-86EE-4F07-B546-D88409547988}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBCD68E-419E-4C6F-ADB8-7AFE4C7C0683}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Company</t>
   </si>
@@ -50,6 +50,39 @@
   </si>
   <si>
     <t>Number of Rating</t>
+  </si>
+  <si>
+    <t>Cosmote</t>
+  </si>
+  <si>
+    <t>COSMOTE</t>
+  </si>
+  <si>
+    <t>ImperiHome</t>
+  </si>
+  <si>
+    <t>Evertygo</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>2.2.0</t>
+  </si>
+  <si>
+    <t>4.7.16</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -372,20 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -393,52 +427,98 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
         <v>4320</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
         <v>891</v>
       </c>
-      <c r="D3" s="2">
-        <v>2</v>
+      <c r="E3" s="2">
+        <v>1.9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
         <v>10018</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>106</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>